<commit_message>
backup: Automate product ID matching and result export
Refactored interliga_bula.py to remove example code and implement real usage: loads product and reference tables, matches IDs, and exports results to resultado_final.xlsx. Added produtos.xlsx as input and updated bula.xlsx.
</commit_message>
<xml_diff>
--- a/bula.xlsx
+++ b/bula.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b84faf9cfcaf1ca1/Documentos/GitHub/VetData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="770" documentId="11_F25DC773A252ABDACC1048DC911C6A7A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D2F7954-F592-427E-BD0C-43E25CEC079C}"/>
+  <xr:revisionPtr revIDLastSave="772" documentId="11_F25DC773A252ABDACC1048DC911C6A7A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D5E755B-FCA1-4760-A29C-8D13D5217FAB}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -801,6 +801,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1532,8 +1536,8 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:J102"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Remove interliga_bula.py and update bula.xlsx
Deleted the interliga_bula.py script
</commit_message>
<xml_diff>
--- a/bula.xlsx
+++ b/bula.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b84faf9cfcaf1ca1/Documentos/GitHub/VetData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="772" documentId="11_F25DC773A252ABDACC1048DC911C6A7A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D5E755B-FCA1-4760-A29C-8D13D5217FAB}"/>
+  <xr:revisionPtr revIDLastSave="774" documentId="11_F25DC773A252ABDACC1048DC911C6A7A5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90D7438B-F002-47E3-A0FD-7ED59BBE3FEC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
-    <sheet name="Planilha2" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -801,10 +801,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1084,454 +1080,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:F21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.90625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-    <col min="6" max="6" width="28.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8123E919-E803-45AF-B028-E68D94DE53D6}">
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:J102"/>
@@ -5126,6 +4674,454 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Planilha1"/>
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.90625" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" customWidth="1"/>
+    <col min="6" max="6" width="28.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE887382-679D-45E5-B4B4-ACC911B0CF70}">
   <sheetPr codeName="Planilha3"/>

</xml_diff>